<commit_message>
Updated Excel command list
</commit_message>
<xml_diff>
--- a/Arduino/Lipsync-Commands.xlsx
+++ b/Arduino/Lipsync-Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\MMC-Github\LipSync-Commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E043DEE1-6774-44FA-ACC1-4AE707C8B8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A90776-A7AC-459A-AC7B-06448FBB4018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4026" yWindow="354" windowWidth="14400" windowHeight="8796" xr2:uid="{217D8EC7-81FA-4179-821A-032DE2A6747B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="2" xr2:uid="{217D8EC7-81FA-4179-821A-032DE2A6747B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouse" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="144">
   <si>
     <t xml:space="preserve">Command </t>
   </si>
@@ -439,9 +439,6 @@
     <t>SUCCESS:BT,1:{Bluetooth Module Mode}</t>
   </si>
   <si>
-    <t>BT,1:{N}</t>
-  </si>
-  <si>
     <t>Set Bluetooth module mode (0=Mouse,1=Keyboard,2=Joystick,3=Mouse and Keyboard)</t>
   </si>
   <si>
@@ -449,6 +446,27 @@
   </si>
   <si>
     <t>RAW:1:{x,y,action}:{xHigh,xLow,yHigh,yLow}</t>
+  </si>
+  <si>
+    <t>BT,1:3</t>
+  </si>
+  <si>
+    <t>CM,0:0</t>
+  </si>
+  <si>
+    <t>SUCCESS:CM,0:{N}</t>
+  </si>
+  <si>
+    <t>Get Communication mode (0=USB , Bluetooth =1)</t>
+  </si>
+  <si>
+    <t>CM,1:{N}</t>
+  </si>
+  <si>
+    <t>SUCCESS:CM,1:{N}</t>
+  </si>
+  <si>
+    <t>Set Communication mode (0=USB , Bluetooth =1)</t>
   </si>
 </sst>
 </file>
@@ -808,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F88DA-293F-41F5-B29B-6468C68A7975}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1086,7 +1104,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1313,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F44C540-4350-4C2F-A574-E1B37A80BDE1}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1591,7 +1609,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1903,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885DA47D-83DD-4CD0-85EF-2B5C8667B129}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2183,7 +2201,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -2389,44 +2407,72 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Arduino code and command instructions
</commit_message>
<xml_diff>
--- a/Arduino/Lipsync-Commands.xlsx
+++ b/Arduino/Lipsync-Commands.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\MMC-Github\LipSync-Commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A90776-A7AC-459A-AC7B-06448FBB4018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C9FD6D-EEB1-4421-9110-073F3A09EAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="2" xr2:uid="{217D8EC7-81FA-4179-821A-032DE2A6747B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="3" xr2:uid="{217D8EC7-81FA-4179-821A-032DE2A6747B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouse" sheetId="1" r:id="rId1"/>
     <sheet name="Gaming" sheetId="2" r:id="rId2"/>
     <sheet name="Wireless" sheetId="3" r:id="rId3"/>
+    <sheet name="Macro" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="147">
   <si>
     <t xml:space="preserve">Command </t>
   </si>
@@ -467,6 +468,15 @@
   </si>
   <si>
     <t>Set Communication mode (0=USB , Bluetooth =1)</t>
+  </si>
+  <si>
+    <t>SUCCESS:MN,0:4</t>
+  </si>
+  <si>
+    <t>Get Model number (4=Macro)</t>
+  </si>
+  <si>
+    <t>BT,1:1</t>
   </si>
 </sst>
 </file>
@@ -1331,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F44C540-4350-4C2F-A574-E1B37A80BDE1}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1923,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885DA47D-83DD-4CD0-85EF-2B5C8667B129}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E45" sqref="A1:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2480,4 +2490,565 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F194DD-AFF3-4759-9926-6C06AC2C4BE0}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="24.41796875" customWidth="1"/>
+    <col min="2" max="2" width="32.3671875" customWidth="1"/>
+    <col min="3" max="3" width="16.62890625" customWidth="1"/>
+    <col min="4" max="4" width="24.734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated gaming firmware and updated documents
</commit_message>
<xml_diff>
--- a/Arduino/Lipsync-Commands.xlsx
+++ b/Arduino/Lipsync-Commands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\MMC-Github\LipSync-Commands\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\AndroidProjects\LipSyncConnect\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C9FD6D-EEB1-4421-9110-073F3A09EAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E942329-ABA5-49C1-8978-DF51CB57ADB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="3" xr2:uid="{217D8EC7-81FA-4179-821A-032DE2A6747B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="150">
   <si>
     <t xml:space="preserve">Command </t>
   </si>
@@ -263,18 +263,6 @@
     <t>SUCCESS:DM,1:1</t>
   </si>
   <si>
-    <t>Get deadzone value (Deadzone Value 1 to 99)</t>
-  </si>
-  <si>
-    <t>Set deadzone value (Deadzone 1 to 99)</t>
-  </si>
-  <si>
-    <t>SUCCESS:DZ,0:{Deadzone Value 1 to 99}</t>
-  </si>
-  <si>
-    <t>SUCCESS:DZ,1:{Deadzone Value 1 to 99}</t>
-  </si>
-  <si>
     <t>SUCCESS:BM,0:{Button Mode}</t>
   </si>
   <si>
@@ -477,6 +465,27 @@
   </si>
   <si>
     <t>BT,1:1</t>
+  </si>
+  <si>
+    <t>SUCCESS:DZ,0:{Deadzone Value 30 to 99}</t>
+  </si>
+  <si>
+    <t>SUCCESS:DZ,1:{Deadzone Value 30 to 99}</t>
+  </si>
+  <si>
+    <t>Get deadzone value (Deadzone Value 30 to 99)</t>
+  </si>
+  <si>
+    <t>Set deadzone value (Deadzone 30 to 99)</t>
+  </si>
+  <si>
+    <t>CT,0:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get change tolerance values based on max value of FSRs and change tolerance percentage </t>
+  </si>
+  <si>
+    <t>SUCCESS:CT,0:{changePercent, xHighChangeTolerance,xLowChangeTolerance, yHighChangeTolerance,yLowChangeTolerance}</t>
   </si>
 </sst>
 </file>
@@ -834,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F88DA-293F-41F5-B29B-6468C68A7975}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -895,13 +904,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -909,13 +918,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -943,7 +952,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -951,7 +960,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -965,7 +974,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -973,7 +982,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1048,79 +1057,79 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1128,13 +1137,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1142,21 +1151,21 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1247,7 +1256,7 @@
         <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1255,7 +1264,7 @@
         <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1263,7 +1272,7 @@
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1271,7 +1280,7 @@
         <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1279,7 +1288,7 @@
         <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1287,62 +1296,77 @@
         <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
         <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
         <v>35</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>50</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F44C540-4350-4C2F-A574-E1B37A80BDE1}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D24"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1414,13 +1438,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1553,79 +1577,79 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1633,13 +1657,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1647,13 +1671,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1661,13 +1685,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1675,21 +1699,21 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1780,7 +1804,7 @@
         <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1788,7 +1812,7 @@
         <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1796,7 +1820,7 @@
         <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1804,7 +1828,7 @@
         <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1812,7 +1836,7 @@
         <v>67</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1820,7 +1844,7 @@
         <v>62</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1828,7 +1852,7 @@
         <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1842,21 +1866,21 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1864,62 +1888,76 @@
         <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
         <v>94</v>
-      </c>
-      <c r="B47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
         <v>35</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>50</v>
       </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1931,10 +1969,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885DA47D-83DD-4CD0-85EF-2B5C8667B129}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="A1:E45"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1992,13 +2030,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2006,13 +2044,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2040,7 +2078,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2048,7 +2086,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2062,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2070,7 +2108,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2145,79 +2183,79 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2225,13 +2263,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2239,21 +2277,21 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2344,7 +2382,7 @@
         <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2352,7 +2390,7 @@
         <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2360,7 +2398,7 @@
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2368,7 +2406,7 @@
         <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2376,7 +2414,7 @@
         <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2384,104 +2422,118 @@
         <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
         <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
         <v>35</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>50</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2494,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F194DD-AFF3-4759-9926-6C06AC2C4BE0}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2555,13 +2607,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2569,13 +2621,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2603,7 +2655,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2611,7 +2663,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2625,7 +2677,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2633,7 +2685,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2708,79 +2760,79 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2788,13 +2840,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2802,21 +2854,21 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2907,7 +2959,7 @@
         <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2915,7 +2967,7 @@
         <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2923,7 +2975,7 @@
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2931,7 +2983,7 @@
         <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2939,7 +2991,7 @@
         <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2947,104 +2999,118 @@
         <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
         <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
         <v>35</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>50</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>